<commit_message>
Continue correcting SpeciesSeeded status for 2x2 data and delete 04_data-exploration.R script becauseit will be replaced with one to look at climate data
</commit_message>
<xml_diff>
--- a/data/data-wrangling-intermediate/03.2b_edited-species-seeded1_SpeciesSeeded-in-mix-assigned.xlsx
+++ b/data/data-wrangling-intermediate/03.2b_edited-species-seeded1_SpeciesSeeded-in-mix-assigned.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="252" documentId="13_ncr:40009_{4E2DAE92-AEF9-46BE-997C-3D03E1D04585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E5E1FC2-6505-4977-8569-1043D36EF31B}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1843,8 +1843,8 @@
   <dimension ref="A1:G283"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A254" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I276" sqref="I276"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>